<commit_message>
Update result graphs for better visual appearance.
</commit_message>
<xml_diff>
--- a/.results/optimizations/Best_GT650.xlsx
+++ b/.results/optimizations/Best_GT650.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="17175" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="17175" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -2309,11 +2309,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="113030656"/>
-        <c:axId val="113797376"/>
+        <c:axId val="49918464"/>
+        <c:axId val="51947200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="113030656"/>
+        <c:axId val="49918464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2329,10 +2329,10 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="2000"/>
                   <a:t>Kernel</a:t>
                 </a:r>
-                <a:endParaRPr lang="cs-CZ"/>
+                <a:endParaRPr lang="cs-CZ" sz="2000"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2343,16 +2343,16 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
-          <a:bodyPr rot="-3300000" vert="horz"/>
+          <a:bodyPr rot="-5400000" vert="horz"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1500" b="0"/>
             </a:pPr>
             <a:endParaRPr lang="cs-CZ"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113797376"/>
+        <c:crossAx val="51947200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2360,7 +2360,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113797376"/>
+        <c:axId val="51947200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2377,14 +2377,14 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="cs-CZ"/>
+                  <a:rPr lang="cs-CZ" sz="2000"/>
                   <a:t>Speedup </a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="2000"/>
                   <a:t>[1]</a:t>
                 </a:r>
-                <a:endParaRPr lang="cs-CZ"/>
+                <a:endParaRPr lang="cs-CZ" sz="2000"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2395,7 +2395,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113030656"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500"/>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="49918464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2404,6 +2414,16 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000"/>
+          </a:pPr>
+          <a:endParaRPr lang="cs-CZ"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
@@ -4040,11 +4060,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="135812096"/>
-        <c:axId val="113799680"/>
+        <c:axId val="94339584"/>
+        <c:axId val="51949504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="135812096"/>
+        <c:axId val="94339584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4082,7 +4102,7 @@
             <a:endParaRPr lang="cs-CZ"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113799680"/>
+        <c:crossAx val="51949504"/>
         <c:crossesAt val="1.0000000000000002E-2"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4090,7 +4110,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113799680"/>
+        <c:axId val="51949504"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4121,7 +4141,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135812096"/>
+        <c:crossAx val="94339584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4319,11 +4339,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="135812608"/>
-        <c:axId val="96629824"/>
+        <c:axId val="101650944"/>
+        <c:axId val="51951232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="135812608"/>
+        <c:axId val="101650944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4336,21 +4356,32 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2500"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="cs-CZ"/>
+                  <a:rPr lang="cs-CZ" sz="2500"/>
                   <a:t>Threads</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96629824"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000"/>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="51951232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4358,7 +4389,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96629824"/>
+        <c:axId val="51951232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4372,34 +4403,56 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2500"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="cs-CZ"/>
+                  <a:rPr lang="cs-CZ" sz="2500"/>
                   <a:t>Time </a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="2500"/>
                   <a:t>[ms]</a:t>
                 </a:r>
-                <a:endParaRPr lang="cs-CZ"/>
+                <a:endParaRPr lang="cs-CZ" sz="2500"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135812608"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000"/>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="101650944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2500"/>
+          </a:pPr>
+          <a:endParaRPr lang="cs-CZ"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -4743,11 +4796,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="137916416"/>
-        <c:axId val="113797952"/>
+        <c:axId val="102127104"/>
+        <c:axId val="45611776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="137916416"/>
+        <c:axId val="102127104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4760,23 +4813,34 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2500"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="2500"/>
                   <a:t>LWS0</a:t>
                 </a:r>
-                <a:endParaRPr lang="cs-CZ"/>
+                <a:endParaRPr lang="cs-CZ" sz="2500"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113797952"/>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000"/>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="45611776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4784,7 +4848,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113797952"/>
+        <c:axId val="45611776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4798,30 +4862,52 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2500"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="2500"/>
                   <a:t>Time [ms]</a:t>
                 </a:r>
-                <a:endParaRPr lang="cs-CZ"/>
+                <a:endParaRPr lang="cs-CZ" sz="2500"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137916416"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000"/>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="102127104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2500"/>
+          </a:pPr>
+          <a:endParaRPr lang="cs-CZ"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -5472,11 +5558,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="137917952"/>
-        <c:axId val="113801408"/>
+        <c:axId val="102126592"/>
+        <c:axId val="51946048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="137917952"/>
+        <c:axId val="102126592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5489,10 +5575,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2500"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="cs-CZ"/>
+                  <a:rPr lang="cs-CZ" sz="2500"/>
                   <a:t>LWS0</a:t>
                 </a:r>
               </a:p>
@@ -5505,7 +5591,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113801408"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000"/>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="51946048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5513,7 +5609,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113801408"/>
+        <c:axId val="51946048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5527,21 +5623,21 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2500"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="cs-CZ"/>
+                  <a:rPr lang="cs-CZ" sz="2500"/>
                   <a:t>Time</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="cs-CZ" baseline="0"/>
+                  <a:rPr lang="cs-CZ" sz="2500" baseline="0"/>
                   <a:t> </a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" sz="2500" baseline="0"/>
                   <a:t>[ms]</a:t>
                 </a:r>
-                <a:endParaRPr lang="cs-CZ"/>
+                <a:endParaRPr lang="cs-CZ" sz="2500"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -5552,7 +5648,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137917952"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000"/>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="102126592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5561,6 +5667,16 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2500"/>
+          </a:pPr>
+          <a:endParaRPr lang="cs-CZ"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -5754,12 +5870,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.92178</cdr:x>
-      <cdr:y>0.28348</cdr:y>
+      <cdr:x>0.88842</cdr:x>
+      <cdr:y>0.08315</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.98586</cdr:x>
-      <cdr:y>0.34207</cdr:y>
+      <cdr:x>0.9885</cdr:x>
+      <cdr:y>0.17954</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -5768,8 +5884,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="7632300" y="1428750"/>
-          <a:ext cx="530625" cy="295275"/>
+          <a:off x="7356085" y="419098"/>
+          <a:ext cx="828665" cy="485778"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -5780,10 +5896,10 @@
         <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:rPr lang="en-US" sz="2500" b="1"/>
             <a:t>LWS1</a:t>
           </a:r>
-          <a:endParaRPr lang="cs-CZ" sz="1100" b="1"/>
+          <a:endParaRPr lang="cs-CZ" sz="2500" b="1"/>
         </a:p>
       </cdr:txBody>
     </cdr:sp>
@@ -9325,7 +9441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -10376,7 +10492,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10390,7 +10506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
@@ -10406,7 +10522,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10421,7 +10537,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>